<commit_message>
added browser parameterization from global datatable and updated test data accordingly
</commit_message>
<xml_diff>
--- a/Chronos/AddNewTimeEntry/testdata.xlsx
+++ b/Chronos/AddNewTimeEntry/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredquentin.hickam\Documents\Unified Functional Testing\ChronosRepo\Chronos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredquentin.hickam\Documents\Unified Functional Testing\ChronosRepo\Chronos\AddNewTimeEntry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
-  <si>
-    <t>Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Hours</t>
   </si>
@@ -87,6 +84,18 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>FIREFOX</t>
   </si>
 </sst>
 </file>
@@ -417,7 +426,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,202 +441,202 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>42968</v>
+      <c r="A2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>42969</v>
+      <c r="A3" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>42969</v>
+      <c r="A4" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>42970</v>
+      <c r="A5" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>42971</v>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>42972</v>
+      <c r="A7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7">
         <v>25</v>

</xml_diff>